<commit_message>
Stinger and Febreze update code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/oxo/OxoTestData.xlsx
+++ b/src/test/resources/TestData/oxo/OxoTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08595E5A-B503-46CF-94C3-984347B85535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF728C8-F8ED-0B4C-880E-C02C3F9E8441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="571" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" tabRatio="571" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
   <si>
     <t>UserName</t>
   </si>
@@ -253,6 +253,9 @@
     <t>OrderID</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>InvalidPaymentDetails</t>
   </si>
   <si>
@@ -322,6 +325,9 @@
     <t>Maryland</t>
   </si>
   <si>
+    <t>100845622</t>
+  </si>
+  <si>
     <t>EmployeeDiscount</t>
   </si>
   <si>
@@ -331,6 +337,18 @@
     <t>NoTaxAddress</t>
   </si>
   <si>
+    <t>6303 Main St Apt B</t>
+  </si>
+  <si>
+    <t>New Port Richey</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>34653</t>
+  </si>
+  <si>
     <t>Akhil@97</t>
   </si>
   <si>
@@ -413,48 +431,6 @@
   </si>
   <si>
     <t>mail</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Provincce</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>prasad.polsani@gmail.com</t>
-  </si>
-  <si>
-    <t>Store</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>100877621</t>
-  </si>
-  <si>
-    <t>Email1</t>
-  </si>
-  <si>
-    <t>Password1</t>
-  </si>
-  <si>
-    <t>QAtest@123</t>
-  </si>
-  <si>
-    <t>PO Box 26321</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>20001</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
   </si>
 </sst>
 </file>
@@ -464,7 +440,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -547,7 +523,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -829,57 +804,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX28"/>
+  <dimension ref="A1:AT28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="AW6" sqref="AW6:AX6"/>
+      <selection activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="29" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="69.85546875" style="12" customWidth="1"/>
-    <col min="35" max="35" width="65.140625" customWidth="1"/>
-    <col min="36" max="36" width="92.42578125" style="12" customWidth="1"/>
-    <col min="37" max="37" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="89.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="69.83203125" style="12" customWidth="1"/>
+    <col min="35" max="35" width="65.1640625" customWidth="1"/>
+    <col min="36" max="36" width="92.5" style="12" customWidth="1"/>
+    <col min="37" max="37" width="44.5" style="12" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="51" customWidth="1"/>
-    <col min="39" max="39" width="33.42578125" customWidth="1"/>
-    <col min="40" max="40" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.5" customWidth="1"/>
+    <col min="40" max="40" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="99.1640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="222" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -935,7 +907,7 @@
         <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>40</v>
@@ -971,95 +943,77 @@
         <v>76</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH1" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AJ1" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AK1" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="AW2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50">
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1068,10 +1022,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -1089,7 +1043,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +1065,7 @@
       </c>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1120,10 +1074,10 @@
         <v>30</v>
       </c>
       <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
@@ -1145,46 +1099,40 @@
         <v>8500563032</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="J6" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>143</v>
+        <v>107</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="M6" s="4">
         <v>9898989898</v>
       </c>
-      <c r="AW6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AX6" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50">
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1192,7 +1140,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -1210,27 +1158,27 @@
         <v>9998999999</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L8">
         <v>21740</v>
@@ -1239,7 +1187,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1254,15 +1202,15 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G10" s="1"/>
       <c r="T10" t="s">
@@ -1278,29 +1226,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1320,7 +1268,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1340,7 +1288,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1360,7 +1308,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1368,66 +1316,60 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F16" s="1"/>
       <c r="AQ16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR16" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT16" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>125</v>
       </c>
-      <c r="AR16" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS16" t="s">
+      <c r="AP17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="AP19" t="s">
         <v>128</v>
       </c>
-      <c r="AT16" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:48">
-      <c r="A17" t="s">
-        <v>119</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:48">
-      <c r="A18" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:48">
-      <c r="A19" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:48">
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" t="s">
-        <v>96</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="I20" t="s">
         <v>25</v>
@@ -1454,41 +1396,26 @@
         <v>65</v>
       </c>
       <c r="AA20" s="8" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="AB20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AC20" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF20" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:48">
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:48">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>69</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I22" t="s">
         <v>72</v>
@@ -1509,90 +1436,90 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:48">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
       <c r="AD23" s="8" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="AE23" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:48">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N24" t="s">
         <v>57</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P24">
         <v>2026</v>
       </c>
       <c r="Q24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R24">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:48">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O25" s="8"/>
       <c r="S25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AO25" s="12"/>
     </row>
-    <row r="26" spans="1:48">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:48">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AG27" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:48" ht="330">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" ht="304" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AH28" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ28" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AI28" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ28" s="12" t="s">
-        <v>90</v>
-      </c>
       <c r="AK28" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL28" s="12" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="AM28" s="12" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AN28" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AO28" s="12" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1608,23 +1535,18 @@
     <hyperlink ref="C11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="F11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F21" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="AF23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B2" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C6" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F3" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="AT16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F20" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="AF20" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="AW2" r:id="rId23" xr:uid="{89A656F7-9B52-418C-8C75-81E18D1636E7}"/>
-    <hyperlink ref="AX2" r:id="rId24" xr:uid="{2FE5B1E5-DF21-4CF5-9D07-3809918DA74C}"/>
-    <hyperlink ref="AW6" r:id="rId25" xr:uid="{84579FDF-32F7-4209-A73D-37E3B8F7E8A6}"/>
-    <hyperlink ref="AX6" r:id="rId26" xr:uid="{F56AC729-6429-4461-AE83-7783EE080F77}"/>
+    <hyperlink ref="F20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AF23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F8" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B2" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F6" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F3" r:id="rId20" xr:uid="{602918C5-1658-4904-89B3-1A9AC410FE96}"/>
+    <hyperlink ref="AT16" r:id="rId21" xr:uid="{4D79D8C6-FFB4-FE45-A365-C2E462DA3255}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>